<commit_message>
Solve the problem of wrong row number in pandas-schema module
</commit_message>
<xml_diff>
--- a/SalesExpense/static/media/客户档案模板2.xlsx
+++ b/SalesExpense/static/media/客户档案模板2.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1906" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1905" uniqueCount="200">
   <si>
     <t>李鲜</t>
   </si>
@@ -709,10 +709,6 @@
   </si>
   <si>
     <t>心内科</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>测试测试测试测试测试测试测试测试测试测试测试测试测试测试测试</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -1569,7 +1565,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O12" sqref="O12"/>
+      <selection pane="bottomLeft" activeCell="T50" sqref="T50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -4589,9 +4585,7 @@
       <c r="S50" s="9">
         <v>400</v>
       </c>
-      <c r="T50" s="9" t="s">
-        <v>200</v>
-      </c>
+      <c r="T50" s="9"/>
     </row>
     <row r="51" spans="1:20">
       <c r="A51" s="10" t="s">

</xml_diff>

<commit_message>
Add comments on template excel
</commit_message>
<xml_diff>
--- a/SalesExpense/static/media/客户档案模板2.xlsx
+++ b/SalesExpense/static/media/客户档案模板2.xlsx
@@ -30,6 +30,114 @@
     <author>作者</author>
   </authors>
   <commentList>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+医院编码必须是大写H开头跟随9个数字的格式。
+医院编码和医院全称不能出现不一致。
+同一医院全称的省份、是否双Call、医院层级、开户进展必须一致</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+医院编码和医院全称不能出现不一致。
+同一医院全称的省份、是否双Call、医院层级、开户进展必须一致</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+本列只接受标准简写。直辖市名、省份名、自治区名不带“市”、“省”、“xx族自治区”后缀。
+如北京、黑龙江、内蒙古</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+本列只接受A、B、C、D四个选项</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
@@ -55,6 +163,216 @@
           </rPr>
           <t xml:space="preserve">
 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+本列只接受（心内科、神内科、老干科、肾内科、内分泌科、其他科室）6个选项</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+本列可以为空</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+必须为0-62之间的整数</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+必须为0或正整数</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+必须是0或正整数</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+必须是0-100之间的整数
+本列请特别注意不要填小数或百分比
+（如想表达相关病人比例为40%，请填40）</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+必须为0或正整数</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+本列可以为空</t>
         </r>
       </text>
     </comment>
@@ -1565,7 +1883,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T50" sqref="T50"/>
+      <selection pane="bottomLeft" activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>

</xml_diff>